<commit_message>
fixed naca0012, added skf1.1
</commit_message>
<xml_diff>
--- a/Airfoil Database/list_airfoils.xlsx
+++ b/Airfoil Database/list_airfoils.xlsx
@@ -1,22 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20408"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20409"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://gtvault-my.sharepoint.com/personal/hlee981_gatech_edu/Documents/Desktop/Airfoil Database/Paper/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hlee981\OneDrive - Georgia Institute of Technology\Desktop\Airfoil Database\Paper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="145" documentId="8_{12632ECB-33DC-4A31-93CF-A52AA0C9C6CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{4AD7A1D0-869D-41B0-8F62-9EB5DC8CE45D}"/>
+  <xr:revisionPtr revIDLastSave="169" documentId="8_{12632ECB-33DC-4A31-93CF-A52AA0C9C6CE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{77345045-262B-4FFF-9C97-BE45873D496E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="2145" windowHeight="0" xr2:uid="{93C099FC-639E-4F92-AB96-B77E1C5407CC}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="2150" windowHeight="0" xr2:uid="{93C099FC-639E-4F92-AB96-B77E1C5407CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="282" uniqueCount="149">
   <si>
     <t>Airfoil</t>
   </si>
@@ -460,7 +459,31 @@
     <t>SSC-A07</t>
   </si>
   <si>
-    <t>SSC-B08</t>
+    <t>2e6 - 4e6</t>
+  </si>
+  <si>
+    <t>1e6 - 2e6</t>
+  </si>
+  <si>
+    <t>1. Fixed transition</t>
+  </si>
+  <si>
+    <t>SSC-A08</t>
+  </si>
+  <si>
+    <t>Need to do</t>
+  </si>
+  <si>
+    <t>SKF 1.1</t>
+  </si>
+  <si>
+    <t>1. Experiment is w/ Maneuver flap, only baseline is digitized</t>
+  </si>
+  <si>
+    <t>2.2e6, 7e6</t>
+  </si>
+  <si>
+    <t>2.5, 5.0</t>
   </si>
 </sst>
 </file>
@@ -562,7 +585,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -661,6 +684,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="10" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -765,8 +797,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5888382-E306-4124-B037-F25DF94F2412}" name="Table2" displayName="Table2" ref="A1:N32" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
-  <autoFilter ref="A1:N32" xr:uid="{F6B5E2EE-9317-44B1-8CF3-4E0A2296C3E9}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{D5888382-E306-4124-B037-F25DF94F2412}" name="Table2" displayName="Table2" ref="A1:N34" totalsRowShown="0" headerRowDxfId="15" dataDxfId="14">
+  <autoFilter ref="A1:N34" xr:uid="{F6B5E2EE-9317-44B1-8CF3-4E0A2296C3E9}"/>
   <tableColumns count="14">
     <tableColumn id="1" xr3:uid="{675A2719-A377-4BBD-8A71-F7E0420D4A22}" name="Airfoil" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{C62E5BD2-2CE3-4993-898C-4E64598D0B16}" name="A (deg)" dataDxfId="12"/>
@@ -1084,32 +1116,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CB4963D9-C860-49EC-92EF-EA8C9FAB7162}">
-  <dimension ref="A1:S33"/>
+  <dimension ref="A1:S34"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="E29" sqref="E29"/>
+      <selection pane="topRight" activeCell="G41" sqref="G41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.85546875" style="1" customWidth="1"/>
-    <col min="2" max="2" width="24.85546875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.5703125" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.42578125" style="1" customWidth="1"/>
-    <col min="5" max="5" width="18.140625" style="1" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" style="1" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="16.5703125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" style="1" customWidth="1"/>
-    <col min="9" max="9" width="17.42578125" style="1" customWidth="1"/>
-    <col min="10" max="10" width="16.5703125" style="1" hidden="1" customWidth="1"/>
-    <col min="11" max="12" width="16.5703125" style="1" customWidth="1"/>
-    <col min="13" max="13" width="18.140625" style="1" customWidth="1"/>
-    <col min="14" max="14" width="46.140625" customWidth="1"/>
+    <col min="1" max="1" width="25.81640625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="24.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="16.54296875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="21.453125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="18.1796875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="16.54296875" style="1" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="16.54296875" style="1" customWidth="1"/>
+    <col min="8" max="8" width="32.54296875" style="1" customWidth="1"/>
+    <col min="9" max="9" width="17.453125" style="1" customWidth="1"/>
+    <col min="10" max="10" width="16.54296875" style="1" hidden="1" customWidth="1"/>
+    <col min="11" max="12" width="16.54296875" style="1" customWidth="1"/>
+    <col min="13" max="13" width="18.1796875" style="1" customWidth="1"/>
+    <col min="14" max="14" width="46.1796875" customWidth="1"/>
     <col min="16" max="16" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1156,7 +1188,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="2" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A2" s="11" t="s">
         <v>7</v>
       </c>
@@ -1193,10 +1225,10 @@
       <c r="N2" s="15"/>
       <c r="P2" s="14">
         <f>SUM(G:G)</f>
-        <v>1305</v>
-      </c>
-    </row>
-    <row r="3" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.25">
+        <v>1307</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="11" t="s">
         <v>8</v>
       </c>
@@ -1232,7 +1264,7 @@
       </c>
       <c r="N3" s="15"/>
     </row>
-    <row r="4" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
@@ -1270,7 +1302,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
@@ -1318,7 +1350,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="31" t="s">
         <v>15</v>
       </c>
@@ -1360,7 +1392,7 @@
         <v>3000000</v>
       </c>
     </row>
-    <row r="7" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="31" t="s">
         <v>23</v>
       </c>
@@ -1403,7 +1435,7 @@
         <v>1.0265523532247542</v>
       </c>
     </row>
-    <row r="8" spans="1:19" s="14" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:19" s="14" customFormat="1" ht="58" x14ac:dyDescent="0.35">
       <c r="A8" s="11" t="s">
         <v>24</v>
       </c>
@@ -1441,7 +1473,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="9" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A9" s="11" t="s">
         <v>24</v>
       </c>
@@ -1477,7 +1509,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="10" spans="1:19" s="14" customFormat="1" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:19" s="14" customFormat="1" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A10" s="31" t="s">
         <v>25</v>
       </c>
@@ -1515,7 +1547,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="11" t="s">
         <v>26</v>
       </c>
@@ -1553,7 +1585,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:19" ht="45" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:19" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A12" s="9" t="s">
         <v>28</v>
       </c>
@@ -1589,7 +1621,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:19" ht="30" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:19" ht="29" x14ac:dyDescent="0.35">
       <c r="A13" s="9" t="s">
         <v>79</v>
       </c>
@@ -1625,7 +1657,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="14" spans="1:19" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:19" s="14" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A14" s="11" t="s">
         <v>29</v>
       </c>
@@ -1663,7 +1695,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="15" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="11" t="s">
         <v>30</v>
       </c>
@@ -1699,7 +1731,7 @@
       </c>
       <c r="N15" s="15"/>
     </row>
-    <row r="16" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:19" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="11" t="s">
         <v>31</v>
       </c>
@@ -1735,7 +1767,7 @@
       </c>
       <c r="N16" s="15"/>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="9" t="s">
         <v>32</v>
       </c>
@@ -1771,7 +1803,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="18" spans="1:14" s="14" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" s="14" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A18" s="11" t="s">
         <v>33</v>
       </c>
@@ -1782,7 +1814,7 @@
         <v>68</v>
       </c>
       <c r="D18" s="11" t="s">
-        <v>14</v>
+        <v>140</v>
       </c>
       <c r="E18" s="11" t="s">
         <v>69</v>
@@ -1809,7 +1841,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A19" s="11" t="s">
         <v>66</v>
       </c>
@@ -1819,7 +1851,9 @@
       <c r="C19" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="D19" s="11"/>
+      <c r="D19" s="11" t="s">
+        <v>141</v>
+      </c>
       <c r="E19" s="11" t="s">
         <v>70</v>
       </c>
@@ -1845,41 +1879,43 @@
         <v>71</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A20" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="B20" s="10" t="s">
+      <c r="B20" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="C20" s="11" t="s">
+      <c r="C20" s="22" t="s">
         <v>74</v>
       </c>
-      <c r="D20" s="12">
+      <c r="D20" s="37">
         <v>6000000</v>
       </c>
-      <c r="E20" s="34">
+      <c r="E20" s="38">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="F20" s="11"/>
-      <c r="G20" s="11"/>
-      <c r="H20" s="11" t="s">
+      <c r="F20" s="22"/>
+      <c r="G20" s="22"/>
+      <c r="H20" s="22" t="s">
         <v>64</v>
       </c>
-      <c r="I20" s="13"/>
-      <c r="J20" s="11"/>
-      <c r="K20" s="11" t="s">
+      <c r="I20" s="24"/>
+      <c r="J20" s="22"/>
+      <c r="K20" s="22" t="s">
         <v>109</v>
       </c>
-      <c r="L20" s="11" t="s">
+      <c r="L20" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="M20" s="11" t="s">
+      <c r="M20" s="22" t="s">
         <v>102</v>
       </c>
-      <c r="N20" s="15"/>
-    </row>
-    <row r="21" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="N20" s="25" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A21" s="11" t="s">
         <v>76</v>
       </c>
@@ -1915,7 +1951,7 @@
       </c>
       <c r="N21" s="15"/>
     </row>
-    <row r="22" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="11" t="s">
         <v>80</v>
       </c>
@@ -1951,7 +1987,7 @@
       </c>
       <c r="N22" s="15"/>
     </row>
-    <row r="23" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
         <v>85</v>
       </c>
@@ -1987,7 +2023,7 @@
       </c>
       <c r="N23" s="25"/>
     </row>
-    <row r="24" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="11" t="s">
         <v>90</v>
       </c>
@@ -2023,7 +2059,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A25" s="11" t="s">
         <v>91</v>
       </c>
@@ -2059,7 +2095,7 @@
       </c>
       <c r="N25" s="15"/>
     </row>
-    <row r="26" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="11" t="s">
         <v>96</v>
       </c>
@@ -2093,7 +2129,7 @@
       </c>
       <c r="N26" s="15"/>
     </row>
-    <row r="27" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A27" s="11" t="s">
         <v>111</v>
       </c>
@@ -2129,7 +2165,7 @@
       </c>
       <c r="N27" s="15"/>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>114</v>
       </c>
@@ -2160,7 +2196,7 @@
       </c>
       <c r="N28" s="6"/>
     </row>
-    <row r="29" spans="1:14" s="11" customFormat="1" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="11" customFormat="1" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="11" t="s">
         <v>116</v>
       </c>
@@ -2196,7 +2232,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="11" t="s">
         <v>119</v>
       </c>
@@ -2232,7 +2268,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="11" t="s">
         <v>123</v>
       </c>
@@ -2265,7 +2301,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A32" s="11" t="s">
         <v>139</v>
       </c>
@@ -2301,9 +2337,54 @@
       </c>
       <c r="N32" s="15"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
-        <v>140</v>
+        <v>143</v>
+      </c>
+      <c r="B33" s="19" t="s">
+        <v>144</v>
+      </c>
+      <c r="C33" s="19"/>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11"/>
+      <c r="N33" s="6"/>
+    </row>
+    <row r="34" spans="1:14" s="14" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="11" t="s">
+        <v>145</v>
+      </c>
+      <c r="B34" s="30" t="s">
+        <v>148</v>
+      </c>
+      <c r="C34" s="30">
+        <v>0.76</v>
+      </c>
+      <c r="D34" s="11" t="s">
+        <v>147</v>
+      </c>
+      <c r="E34" s="17">
+        <v>0.01</v>
+      </c>
+      <c r="F34" s="11"/>
+      <c r="G34" s="11">
+        <v>2</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="I34" s="11"/>
+      <c r="J34" s="11"/>
+      <c r="K34" s="11" t="s">
+        <v>109</v>
+      </c>
+      <c r="L34" s="11" t="s">
+        <v>104</v>
+      </c>
+      <c r="M34" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="N34" s="15" t="s">
+        <v>146</v>
       </c>
     </row>
   </sheetData>
@@ -2563,20 +2644,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="d624ff89-a3d8-48ad-8a73-6b7263eb58d2" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="d624ff89-a3d8-48ad-8a73-6b7263eb58d2" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2599,26 +2680,26 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{643E2EEA-CCBB-4A59-A4B0-FBA954000719}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E361C660-8B5A-497A-AEA7-466AA4F145C4}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="d624ff89-a3d8-48ad-8a73-6b7263eb58d2"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="caebe9e7-4d6b-4886-b893-b59babeb2752"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E361C660-8B5A-497A-AEA7-466AA4F145C4}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{643E2EEA-CCBB-4A59-A4B0-FBA954000719}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="caebe9e7-4d6b-4886-b893-b59babeb2752"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="d624ff89-a3d8-48ad-8a73-6b7263eb58d2"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
adding naca 45-100, Mustang wing
</commit_message>
<xml_diff>
--- a/Airfoil Database/list_airfoils.xlsx
+++ b/Airfoil Database/list_airfoils.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Cloned Respositories\GP-Aero\Airfoil Database\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3048C918-42C9-48AC-A0E6-6FCF3E152453}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{557B928D-3808-46B0-9FEB-9219F97F8476}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="244">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="248">
   <si>
     <t>Airfoil</t>
   </si>
@@ -425,9 +425,6 @@
     <t>MBB</t>
   </si>
   <si>
-    <t>1. Did only up to p 295</t>
-  </si>
-  <si>
     <t>Supercritical airfoil 9a</t>
   </si>
   <si>
@@ -477,9 +474,6 @@
   </si>
   <si>
     <t>NACA TM 100526</t>
-  </si>
-  <si>
-    <t>Wing</t>
   </si>
   <si>
     <t>SSC-A09</t>
@@ -771,13 +765,31 @@
   </si>
   <si>
     <t>Shifted by 1.0</t>
+  </si>
+  <si>
+    <t>1. Did only up to p 295 (Results from ARA Bedford Tunnel)</t>
+  </si>
+  <si>
+    <t>NACA 45-100</t>
+  </si>
+  <si>
+    <t>Interpolated results discretized into provided pressure tap locations</t>
+  </si>
+  <si>
+    <t>R &amp; M No. 2251</t>
+  </si>
+  <si>
+    <t>0.4 - 0.775</t>
+  </si>
+  <si>
+    <t>will be filled in</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="24" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -958,8 +970,31 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="4"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -982,6 +1017,11 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF000000"/>
         <bgColor rgb="FF202124"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -1048,14 +1088,15 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="5">
+  <cellStyleXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="14" fillId="3" borderId="0" applyBorder="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" applyBorder="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1210,11 +1251,18 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="2" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="0" xfId="5" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="5">
+  <cellStyles count="6">
     <cellStyle name="Excel Built-in Good" xfId="2" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
     <cellStyle name="Excel Built-in Good 1" xfId="4" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
     <cellStyle name="Excel Built-in Neutral" xfId="3" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="Neutral" xfId="5" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
   </cellStyles>
@@ -1622,10 +1670,10 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
       <selection activeCell="A30" sqref="A30"/>
-      <selection pane="topRight" activeCell="O51" sqref="O51"/>
+      <selection pane="topRight" activeCell="K54" sqref="K54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1739,7 +1787,7 @@
       <c r="O2" s="10"/>
       <c r="Q2" s="11">
         <f>SUM(G2:G11,G14:G16,G18:G22,G24:G65)</f>
-        <v>1570</v>
+        <v>1572</v>
       </c>
     </row>
     <row r="3" spans="1:20" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
@@ -2693,7 +2741,7 @@
       <c r="O23" s="27"/>
     </row>
     <row r="24" spans="1:15" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A24" s="4" t="s">
+      <c r="A24" s="54" t="s">
         <v>123</v>
       </c>
       <c r="B24" s="4" t="s">
@@ -2702,7 +2750,9 @@
       <c r="C24" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="D24" s="4"/>
+      <c r="D24" s="5">
+        <v>6000000</v>
+      </c>
       <c r="E24" s="31" t="s">
         <v>126</v>
       </c>
@@ -2710,7 +2760,7 @@
         <v>94</v>
       </c>
       <c r="G24" s="4">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="H24" s="8"/>
       <c r="I24" s="4" t="s">
@@ -2732,24 +2782,24 @@
         <v>25</v>
       </c>
       <c r="O24" s="10" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A25" s="54" t="s">
         <v>129</v>
       </c>
-    </row>
-    <row r="25" spans="1:15" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A25" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>130</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>131</v>
       </c>
       <c r="C25" s="4" t="s">
         <v>104</v>
       </c>
       <c r="D25" s="4" t="s">
+        <v>131</v>
+      </c>
+      <c r="E25" s="32" t="s">
         <v>132</v>
-      </c>
-      <c r="E25" s="32" t="s">
-        <v>133</v>
       </c>
       <c r="F25" s="7" t="s">
         <v>94</v>
@@ -2768,10 +2818,10 @@
         <v>29</v>
       </c>
       <c r="L25" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="M25" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="M25" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="N25" s="4" t="s">
         <v>25</v>
@@ -2780,22 +2830,22 @@
     </row>
     <row r="26" spans="1:15" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A26" s="33" t="s">
+        <v>135</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>136</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="D26" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>139</v>
       </c>
       <c r="E26" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F26" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G26" s="4">
         <v>18</v>
@@ -2811,10 +2861,10 @@
         <v>29</v>
       </c>
       <c r="L26" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="M26" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="M26" s="4" t="s">
-        <v>142</v>
       </c>
       <c r="N26" s="4" t="s">
         <v>25</v>
@@ -2823,13 +2873,13 @@
     </row>
     <row r="27" spans="1:15" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A27" s="4" t="s">
+        <v>142</v>
+      </c>
+      <c r="B27" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="C27" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="D27" s="5">
         <v>3000000</v>
@@ -2838,14 +2888,14 @@
         <v>21</v>
       </c>
       <c r="F27" s="7" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="G27" s="4">
         <v>66</v>
       </c>
       <c r="H27" s="20"/>
       <c r="I27" s="4" t="s">
-        <v>147</v>
+        <v>20</v>
       </c>
       <c r="J27" s="4" t="s">
         <v>21</v>
@@ -2866,22 +2916,22 @@
     </row>
     <row r="28" spans="1:15" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A28" s="25" t="s">
+        <v>146</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D28" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>149</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D28" s="4" t="s">
-        <v>150</v>
       </c>
       <c r="E28" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F28" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G28" s="4">
         <v>16</v>
@@ -2897,10 +2947,10 @@
         <v>29</v>
       </c>
       <c r="L28" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M28" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N28" s="4" t="s">
         <v>25</v>
@@ -2909,13 +2959,13 @@
     </row>
     <row r="29" spans="1:15" s="34" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A29" s="12" t="s">
+        <v>150</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C29" s="4" t="s">
         <v>152</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>153</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>154</v>
       </c>
       <c r="D29" s="5">
         <v>2000000</v>
@@ -2924,14 +2974,14 @@
         <v>0.03</v>
       </c>
       <c r="F29" s="7" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="G29" s="4">
         <v>7</v>
       </c>
       <c r="H29" s="8"/>
       <c r="I29" s="4" t="s">
-        <v>147</v>
+        <v>20</v>
       </c>
       <c r="J29" s="4" t="s">
         <v>9</v>
@@ -2940,27 +2990,27 @@
         <v>29</v>
       </c>
       <c r="L29" s="4" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="M29" s="4" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="N29" s="4" t="s">
         <v>25</v>
       </c>
       <c r="O29" s="17" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:15" s="11" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A30" s="25" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D30" s="5">
         <v>4400000</v>
@@ -2969,14 +3019,14 @@
         <v>2.5000000000000001E-3</v>
       </c>
       <c r="F30" s="7" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="G30" s="4">
         <v>86</v>
       </c>
       <c r="H30" s="8"/>
       <c r="I30" s="4" t="s">
-        <v>147</v>
+        <v>20</v>
       </c>
       <c r="J30" s="4" t="s">
         <v>9</v>
@@ -2985,36 +3035,36 @@
         <v>29</v>
       </c>
       <c r="L30" s="4" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="M30" s="4" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="N30" s="4" t="s">
         <v>25</v>
       </c>
       <c r="O30" s="17" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
     </row>
     <row r="31" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A31" s="25" t="s">
+        <v>163</v>
+      </c>
+      <c r="B31" s="18" t="s">
+        <v>164</v>
+      </c>
+      <c r="C31" s="4" t="s">
         <v>165</v>
       </c>
-      <c r="B31" s="18" t="s">
+      <c r="D31" s="4" t="s">
         <v>166</v>
-      </c>
-      <c r="C31" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="D31" s="4" t="s">
-        <v>168</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>21</v>
       </c>
       <c r="F31" s="7" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="G31" s="4">
         <v>112</v>
@@ -3030,36 +3080,36 @@
         <v>22</v>
       </c>
       <c r="L31" s="4" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="M31" s="4" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="N31" s="4" t="s">
         <v>25</v>
       </c>
       <c r="O31" s="10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="32" spans="1:15" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A32" s="25" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D32" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E32" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F32" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G32" s="4">
         <v>17</v>
@@ -3075,10 +3125,10 @@
         <v>29</v>
       </c>
       <c r="L32" s="4" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="M32" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N32" s="4" t="s">
         <v>25</v>
@@ -3087,22 +3137,22 @@
     </row>
     <row r="33" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A33" s="25" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D33" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E33" s="18" t="s">
         <v>21</v>
       </c>
       <c r="F33" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G33" s="4">
         <v>18</v>
@@ -3118,30 +3168,30 @@
         <v>29</v>
       </c>
       <c r="L33" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="N33" s="4" t="s">
         <v>25</v>
       </c>
       <c r="O33" s="27" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="34" spans="1:15" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A34" s="25" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C34" s="4">
         <v>0.76</v>
       </c>
       <c r="D34" s="4" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="E34" s="32">
         <v>0.01</v>
@@ -3154,7 +3204,7 @@
       </c>
       <c r="H34" s="8"/>
       <c r="I34" s="4" t="s">
-        <v>147</v>
+        <v>20</v>
       </c>
       <c r="J34" s="4" t="s">
         <v>9</v>
@@ -3166,31 +3216,31 @@
         <v>21</v>
       </c>
       <c r="M34" s="4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="N34" s="4" t="s">
         <v>25</v>
       </c>
       <c r="O34" s="10" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="35" spans="1:15" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A35" s="4" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B35" s="4"/>
       <c r="C35" s="4" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="D35" s="4" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E35" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F35" s="7" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="G35" s="4">
         <v>55</v>
@@ -3206,24 +3256,24 @@
         <v>29</v>
       </c>
       <c r="L35" s="4" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="N35" s="4" t="s">
         <v>25</v>
       </c>
       <c r="O35" s="10" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
     </row>
     <row r="36" spans="1:15" s="34" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A36" s="25" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C36" s="38">
         <v>0.22</v>
@@ -3235,7 +3285,7 @@
         <v>21</v>
       </c>
       <c r="F36" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G36" s="4">
         <v>3</v>
@@ -3251,10 +3301,10 @@
         <v>29</v>
       </c>
       <c r="L36" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="N36" s="4" t="s">
         <v>25</v>
@@ -3263,10 +3313,10 @@
     </row>
     <row r="37" spans="1:15" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A37" s="25" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C37" s="4">
         <v>0.22</v>
@@ -3278,7 +3328,7 @@
         <v>21</v>
       </c>
       <c r="F37" s="7" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="G37" s="4">
         <v>3</v>
@@ -3294,10 +3344,10 @@
         <v>29</v>
       </c>
       <c r="L37" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="N37" s="4" t="s">
         <v>25</v>
@@ -3306,22 +3356,22 @@
     </row>
     <row r="38" spans="1:15" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A38" s="25" t="s">
+        <v>193</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C38" s="4" t="s">
+        <v>137</v>
+      </c>
+      <c r="D38" s="4" t="s">
         <v>195</v>
-      </c>
-      <c r="B38" s="4" t="s">
-        <v>196</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>138</v>
-      </c>
-      <c r="D38" s="4" t="s">
-        <v>197</v>
       </c>
       <c r="E38" s="32">
         <v>0.01</v>
       </c>
       <c r="F38" s="7" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="G38" s="4">
         <v>18</v>
@@ -3337,10 +3387,10 @@
         <v>29</v>
       </c>
       <c r="L38" s="4" t="s">
+        <v>133</v>
+      </c>
+      <c r="M38" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>135</v>
       </c>
       <c r="N38" s="4" t="s">
         <v>25</v>
@@ -3349,22 +3399,22 @@
     </row>
     <row r="39" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A39" s="12" t="s">
+        <v>197</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>198</v>
+      </c>
+      <c r="C39" s="4" t="s">
         <v>199</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="D39" s="4" t="s">
         <v>200</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>201</v>
-      </c>
-      <c r="D39" s="4" t="s">
-        <v>202</v>
       </c>
       <c r="E39" s="4">
         <v>0.08</v>
       </c>
       <c r="F39" s="7" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="G39" s="4">
         <v>6</v>
@@ -3380,24 +3430,24 @@
         <v>29</v>
       </c>
       <c r="L39" s="4" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="M39" s="4" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="N39" s="4" t="s">
         <v>25</v>
       </c>
       <c r="O39" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="40" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A40" s="40" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B40" s="41" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="C40" s="41">
         <v>0.1</v>
@@ -3409,7 +3459,7 @@
         <v>21</v>
       </c>
       <c r="F40" s="7" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="G40" s="41">
         <v>2</v>
@@ -3425,10 +3475,10 @@
         <v>29</v>
       </c>
       <c r="L40" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="M40" s="4" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="N40" s="4" t="s">
         <v>25</v>
@@ -3437,10 +3487,10 @@
     </row>
     <row r="41" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A41" s="40" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B41" s="41" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="C41" s="41">
         <v>0.15</v>
@@ -3452,7 +3502,7 @@
         <v>21</v>
       </c>
       <c r="F41" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G41" s="41">
         <v>6</v>
@@ -3468,10 +3518,10 @@
         <v>29</v>
       </c>
       <c r="L41" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M41" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N41" s="4" t="s">
         <v>25</v>
@@ -3480,10 +3530,10 @@
     </row>
     <row r="42" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A42" s="40" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="B42" s="41" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C42" s="41">
         <v>0.15</v>
@@ -3495,7 +3545,7 @@
         <v>21</v>
       </c>
       <c r="F42" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G42" s="41">
         <v>6</v>
@@ -3511,10 +3561,10 @@
         <v>29</v>
       </c>
       <c r="L42" s="4" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="M42" s="4" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
       <c r="N42" s="4" t="s">
         <v>25</v>
@@ -3523,10 +3573,10 @@
     </row>
     <row r="43" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A43" s="40" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B43" s="41" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C43" s="41">
         <v>0.122</v>
@@ -3538,7 +3588,7 @@
         <v>21</v>
       </c>
       <c r="F43" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G43" s="41">
         <v>6</v>
@@ -3554,10 +3604,10 @@
         <v>29</v>
       </c>
       <c r="L43" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N43" s="4" t="s">
         <v>25</v>
@@ -3566,10 +3616,10 @@
     </row>
     <row r="44" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A44" s="40" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
       <c r="B44" s="41" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="C44" s="41">
         <v>0.122</v>
@@ -3581,7 +3631,7 @@
         <v>21</v>
       </c>
       <c r="F44" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G44" s="41">
         <v>6</v>
@@ -3597,10 +3647,10 @@
         <v>29</v>
       </c>
       <c r="L44" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N44" s="4" t="s">
         <v>25</v>
@@ -3609,10 +3659,10 @@
     </row>
     <row r="45" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A45" s="40" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="B45" s="41" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
       <c r="C45" s="41">
         <v>0.122</v>
@@ -3624,7 +3674,7 @@
         <v>21</v>
       </c>
       <c r="F45" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G45" s="41">
         <v>6</v>
@@ -3640,10 +3690,10 @@
         <v>29</v>
       </c>
       <c r="L45" s="4" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
       <c r="M45" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N45" s="4" t="s">
         <v>25</v>
@@ -3652,10 +3702,10 @@
     </row>
     <row r="46" spans="1:15" s="49" customFormat="1" ht="31" x14ac:dyDescent="0.35">
       <c r="A46" s="44" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="B46" s="45" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="C46" s="44">
         <v>0.09</v>
@@ -3667,7 +3717,7 @@
         <v>21</v>
       </c>
       <c r="F46" s="47" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
       <c r="G46" s="44">
         <v>10</v>
@@ -3683,36 +3733,36 @@
         <v>29</v>
       </c>
       <c r="L46" s="44" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="M46" s="44" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
       <c r="N46" s="44" t="s">
         <v>25</v>
       </c>
       <c r="O46" s="48" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="47" spans="1:15" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A47" s="4" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C47" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D47" s="4" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="E47" s="4" t="s">
         <v>21</v>
       </c>
       <c r="F47" s="7" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="G47" s="4">
         <v>17</v>
@@ -3728,10 +3778,10 @@
         <v>29</v>
       </c>
       <c r="L47" s="4" t="s">
+        <v>140</v>
+      </c>
+      <c r="M47" s="4" t="s">
         <v>141</v>
-      </c>
-      <c r="M47" s="4" t="s">
-        <v>142</v>
       </c>
       <c r="N47" s="4" t="s">
         <v>25</v>
@@ -3740,10 +3790,10 @@
     </row>
     <row r="48" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A48" s="4" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>231</v>
+        <v>229</v>
       </c>
       <c r="C48" s="4">
         <v>0.104</v>
@@ -3755,7 +3805,7 @@
         <v>21</v>
       </c>
       <c r="F48" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G48" s="4">
         <v>6</v>
@@ -3780,15 +3830,15 @@
         <v>25</v>
       </c>
       <c r="O48" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="49" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A49" s="4" t="s">
-        <v>232</v>
+        <v>230</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>233</v>
+        <v>231</v>
       </c>
       <c r="C49" s="4">
         <v>0.106</v>
@@ -3800,7 +3850,7 @@
         <v>21</v>
       </c>
       <c r="F49" s="7" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="G49" s="4">
         <v>6</v>
@@ -3825,12 +3875,12 @@
         <v>25</v>
       </c>
       <c r="O49" s="10" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
     </row>
     <row r="50" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A50" s="4" t="s">
-        <v>234</v>
+        <v>232</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>21</v>
@@ -3845,7 +3895,7 @@
         <v>21</v>
       </c>
       <c r="F50" s="50" t="s">
-        <v>235</v>
+        <v>233</v>
       </c>
       <c r="G50" s="4">
         <v>14</v>
@@ -3861,7 +3911,7 @@
         <v>29</v>
       </c>
       <c r="L50" s="4" t="s">
-        <v>236</v>
+        <v>234</v>
       </c>
       <c r="M50" s="4" t="s">
         <v>24</v>
@@ -3870,15 +3920,15 @@
         <v>25</v>
       </c>
       <c r="O50" s="10" t="s">
-        <v>243</v>
+        <v>241</v>
       </c>
     </row>
     <row r="51" spans="1:15" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A51" s="4" t="s">
-        <v>237</v>
+        <v>235</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C51" s="4">
         <v>0.12</v>
@@ -3890,7 +3940,7 @@
         <v>21</v>
       </c>
       <c r="F51" s="51" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G51" s="4">
         <v>8</v>
@@ -3906,24 +3956,24 @@
         <v>29</v>
       </c>
       <c r="L51" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N51" s="4" t="s">
         <v>25</v>
       </c>
       <c r="O51" s="10" t="s">
-        <v>241</v>
+        <v>239</v>
       </c>
     </row>
     <row r="52" spans="1:15" ht="39.5" x14ac:dyDescent="0.35">
       <c r="A52" s="4" t="s">
-        <v>242</v>
+        <v>240</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>238</v>
+        <v>236</v>
       </c>
       <c r="C52" s="4">
         <v>0.12</v>
@@ -3935,7 +3985,7 @@
         <v>21</v>
       </c>
       <c r="F52" s="51" t="s">
-        <v>239</v>
+        <v>237</v>
       </c>
       <c r="G52" s="4">
         <v>8</v>
@@ -3951,34 +4001,62 @@
         <v>29</v>
       </c>
       <c r="L52" s="4" t="s">
-        <v>240</v>
+        <v>238</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="N52" s="4" t="s">
         <v>25</v>
       </c>
       <c r="O52" s="10" t="s">
-        <v>241</v>
-      </c>
-    </row>
-    <row r="53" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
-      <c r="A53" s="18"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="18"/>
-      <c r="D53" s="18"/>
-      <c r="E53" s="18"/>
-      <c r="F53" s="52"/>
-      <c r="G53" s="18"/>
-      <c r="H53" s="18"/>
-      <c r="I53" s="4"/>
-      <c r="J53" s="4"/>
-      <c r="K53" s="18"/>
-      <c r="L53" s="4"/>
-      <c r="M53" s="4"/>
-      <c r="N53" s="4"/>
-      <c r="O53" s="27"/>
+        <v>239</v>
+      </c>
+    </row>
+    <row r="53" spans="1:15" s="11" customFormat="1" ht="15.5" x14ac:dyDescent="0.35">
+      <c r="A53" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>246</v>
+      </c>
+      <c r="D53" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="E53" s="4" t="s">
+        <v>247</v>
+      </c>
+      <c r="F53" s="51" t="s">
+        <v>245</v>
+      </c>
+      <c r="G53" s="4">
+        <v>3</v>
+      </c>
+      <c r="H53" s="55"/>
+      <c r="I53" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="J53" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="K53" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="L53" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="M53" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="N53" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="O53" s="10" t="s">
+        <v>244</v>
+      </c>
     </row>
     <row r="54" spans="1:15" ht="15.5" x14ac:dyDescent="0.35">
       <c r="A54" s="18"/>
@@ -20081,9 +20159,9 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <tableParts count="1">
-    <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>